<commit_message>
update sampling method lut
</commit_message>
<xml_diff>
--- a/nbs/files/lut/dbo_sampmet.xlsx
+++ b/nbs/files/lut/dbo_sampmet.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27103"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{93059FF6-8156-4708-B2F6-D427D097696E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franckalbinet/pro/IAEA/MARIS/marisco/nbs/files/lut/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655031ED-D29F-E245-A1EF-39AA88E3BC81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="23895" windowHeight="14535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="500" windowWidth="23900" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dbo_sampmet" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="dbo_sampmet">dbo_sampmet!$A$1:$G$27</definedName>
+    <definedName name="dbo_sampmet">dbo_sampmet!$A$1:$G$26</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -32,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>sampmet_id</t>
   </si>
@@ -185,12 +190,6 @@
   </si>
   <si>
     <t>FILT</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>DCN</t>
   </si>
   <si>
     <t>Bucket</t>
@@ -215,11 +214,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="MS Sans Serif"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -264,9 +263,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -304,9 +303,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -339,9 +338,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -374,9 +390,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -550,19 +583,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="47.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="47.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -585,7 +618,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -608,7 +641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -631,7 +664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -654,7 +687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -677,7 +710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -700,7 +733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -723,7 +756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -746,7 +779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -769,7 +802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -792,7 +825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -815,7 +848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -838,7 +871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -861,7 +894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -884,7 +917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -907,7 +940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -930,7 +963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -953,7 +986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -976,7 +1009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -999,7 +1032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1022,7 +1055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1045,7 +1078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1068,7 +1101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1091,9 +1124,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>51</v>
@@ -1102,21 +1135,18 @@
         <v>52</v>
       </c>
       <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
         <v>2</v>
       </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
       <c r="G24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>53</v>
@@ -1128,15 +1158,18 @@
         <v>1</v>
       </c>
       <c r="E25">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
       </c>
       <c r="G25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>55</v>
@@ -1154,29 +1187,6 @@
         <v>0</v>
       </c>
       <c r="G26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
-        <v>57</v>
-      </c>
-      <c r="C27" t="s">
-        <v>58</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-      <c r="G27">
         <v>1</v>
       </c>
     </row>
@@ -1186,26 +1196,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f3c01d95-e195-4940-9fb4-afa395d98e0b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="77012c7d-7b27-41e5-8843-0f8877a4d830" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006C266C02A97D1D41B60FC5BB4AB3B561" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e4b12e3bfb62cc8e0d480f11bb3af7cc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f3c01d95-e195-4940-9fb4-afa395d98e0b" xmlns:ns3="77012c7d-7b27-41e5-8843-0f8877a4d830" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f0b17c4e0e330c3092c651d54c7b73f6" ns2:_="" ns3:_="">
     <xsd:import namespace="f3c01d95-e195-4940-9fb4-afa395d98e0b"/>
@@ -1434,14 +1424,60 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f3c01d95-e195-4940-9fb4-afa395d98e0b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="77012c7d-7b27-41e5-8843-0f8877a4d830" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73383578-630E-4DED-8666-239D2D5F2B23}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{72B71A72-56F7-440A-B31C-07F746B72138}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f3c01d95-e195-4940-9fb4-afa395d98e0b"/>
+    <ds:schemaRef ds:uri="77012c7d-7b27-41e5-8843-0f8877a4d830"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1308EA83-388C-4057-B7FE-29043D757054}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1308EA83-388C-4057-B7FE-29043D757054}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{72B71A72-56F7-440A-B31C-07F746B72138}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73383578-630E-4DED-8666-239D2D5F2B23}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f3c01d95-e195-4940-9fb4-afa395d98e0b"/>
+    <ds:schemaRef ds:uri="77012c7d-7b27-41e5-8843-0f8877a4d830"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>